<commit_message>
Manutenção no processo de exportação da planilha xlsx.
</commit_message>
<xml_diff>
--- a/ProjetoAlgoritmoDeInferencia/Saída/Percentual de similaridade.xlsx
+++ b/ProjetoAlgoritmoDeInferencia/Saída/Percentual de similaridade.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="68">
   <si>
     <t>Resultado da aplicação do algoritmo de cálculo do percentual de similaridade entre os indivíduos</t>
   </si>
@@ -60,6 +60,162 @@
   </si>
   <si>
     <t>SOFTWARE</t>
+  </si>
+  <si>
+    <t>Sergio Antônio Andrade de Freitas</t>
+  </si>
+  <si>
+    <t>Destino 1</t>
+  </si>
+  <si>
+    <t>0395549254894676</t>
+  </si>
+  <si>
+    <t>Andre Luiz Aquere de Cerqueira e Souza</t>
+  </si>
+  <si>
+    <t>Destino 2</t>
+  </si>
+  <si>
+    <t>8424412648258970</t>
+  </si>
+  <si>
+    <t>CIVIL</t>
+  </si>
+  <si>
+    <t>Edson Mintsu Hung Destino</t>
+  </si>
+  <si>
+    <t>Destino 3</t>
+  </si>
+  <si>
+    <t>6753551743147880</t>
+  </si>
+  <si>
+    <t>ELETRÔNICA</t>
+  </si>
+  <si>
+    <t>Edgard Costa Oliveira</t>
+  </si>
+  <si>
+    <t>Destino 4</t>
+  </si>
+  <si>
+    <t>1196380808351110</t>
+  </si>
+  <si>
+    <t>Edson Alves da Costa Júnior</t>
+  </si>
+  <si>
+    <t>Destino 5</t>
+  </si>
+  <si>
+    <t>2105379147123450</t>
+  </si>
+  <si>
+    <t>André Barros de Sales</t>
+  </si>
+  <si>
+    <t>Destino 6</t>
+  </si>
+  <si>
+    <t>7610669796869660</t>
+  </si>
+  <si>
+    <t>Giovanni Almeida dos Santos</t>
+  </si>
+  <si>
+    <t>Destino 7</t>
+  </si>
+  <si>
+    <t>0580891429319047</t>
+  </si>
+  <si>
+    <t>Cristiane Soares Ramos</t>
+  </si>
+  <si>
+    <t>Destino 8</t>
+  </si>
+  <si>
+    <t>9950213660160160</t>
+  </si>
+  <si>
+    <t>Fabricio Ataides Braz</t>
+  </si>
+  <si>
+    <t>Destino 9</t>
+  </si>
+  <si>
+    <t>1700216932505000</t>
+  </si>
+  <si>
+    <t>Alexandre Sérgio de Araújo Bezerra</t>
+  </si>
+  <si>
+    <t>Destino 10</t>
+  </si>
+  <si>
+    <t>0255998976169051</t>
+  </si>
+  <si>
+    <t>MEDICINA</t>
+  </si>
+  <si>
+    <t>Eduardo Stockler Tognetti</t>
+  </si>
+  <si>
+    <t>Destino 11</t>
+  </si>
+  <si>
+    <t>2443108673822680</t>
+  </si>
+  <si>
+    <t>ELÉTRICA</t>
+  </si>
+  <si>
+    <t>Jan Mendonça Correa</t>
+  </si>
+  <si>
+    <t>Destino 12</t>
+  </si>
+  <si>
+    <t>7844006017790570</t>
+  </si>
+  <si>
+    <t>CIÊNCIA DA COMPUTAÇÃO</t>
+  </si>
+  <si>
+    <t>Rejane Maria da Costa Figueiredo</t>
+  </si>
+  <si>
+    <t>Destino 13</t>
+  </si>
+  <si>
+    <t>2187680174312042</t>
+  </si>
+  <si>
+    <t>Augusto César de Mendonça Brasil</t>
+  </si>
+  <si>
+    <t>Destino 14</t>
+  </si>
+  <si>
+    <t>0571960641751286</t>
+  </si>
+  <si>
+    <t>ENERGIA</t>
+  </si>
+  <si>
+    <t>Fábio Macêdo Mendes</t>
+  </si>
+  <si>
+    <t>Destino 15</t>
+  </si>
+  <si>
+    <t>8075435338067780</t>
+  </si>
+  <si>
+    <t>FÍSICA</t>
   </si>
 </sst>
 </file>
@@ -82,13 +238,13 @@
     </font>
     <font>
       <name val="Calibri"/>
-      <sz val="11.0"/>
+      <sz val="10.0"/>
       <color indexed="9"/>
       <b val="true"/>
     </font>
     <font>
       <name val="Calibri"/>
-      <sz val="11.0"/>
+      <sz val="10.0"/>
       <color indexed="9"/>
       <b val="true"/>
     </font>
@@ -217,19 +373,19 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment horizontal="center" vertical="center" wrapText="true"/>
+      <alignment horizontal="left" vertical="center" wrapText="true"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment horizontal="center" vertical="center" wrapText="true"/>
+      <alignment horizontal="left" vertical="center" wrapText="true"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="true">
-      <alignment horizontal="center" wrapText="true"/>
+      <alignment horizontal="left" wrapText="true"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true" applyNumberFormat="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true" applyNumberFormat="true">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
 </styleSheet>
@@ -246,15 +402,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="30.0" customWidth="true"/>
-    <col min="2" max="2" width="20.0" customWidth="true"/>
+    <col min="1" max="1" width="2.0" customWidth="true"/>
+    <col min="2" max="2" width="24.0" customWidth="true"/>
     <col min="3" max="3" width="20.0" customWidth="true"/>
-    <col min="4" max="4" width="20.0" customWidth="true"/>
+    <col min="4" max="4" width="18.0" customWidth="true"/>
     <col min="5" max="5" width="20.0" customWidth="true"/>
-    <col min="6" max="6" width="20.0" customWidth="true"/>
-    <col min="7" max="7" width="20.0" customWidth="true"/>
-    <col min="8" max="8" width="20.0" customWidth="true"/>
-    <col min="9" max="9" width="20.0" customWidth="true"/>
+    <col min="6" max="6" width="15.0" customWidth="true"/>
+    <col min="7" max="7" width="15.0" customWidth="true"/>
+    <col min="8" max="8" width="15.0" customWidth="true"/>
+    <col min="9" max="9" width="15.0" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.0" customHeight="true">
@@ -263,63 +419,377 @@
       </c>
     </row>
     <row r="2" ht="15.0" customHeight="true">
-      <c r="A2" t="s" s="2">
+      <c r="B2" t="s" s="2">
         <v>1</v>
       </c>
-      <c r="B2" t="s" s="2">
+      <c r="C2" t="s" s="2">
         <v>2</v>
       </c>
-      <c r="C2" t="s" s="2">
+      <c r="D2" t="s" s="2">
         <v>3</v>
       </c>
-      <c r="D2" t="s" s="2">
+      <c r="E2" t="s" s="2">
         <v>4</v>
       </c>
-      <c r="E2" t="s" s="2">
+      <c r="F2" t="s" s="2">
         <v>5</v>
       </c>
-      <c r="F2" t="s" s="2">
+      <c r="G2" t="s" s="2">
         <v>6</v>
       </c>
-      <c r="G2" t="s" s="2">
+      <c r="H2" t="s" s="2">
         <v>7</v>
       </c>
     </row>
     <row r="3" ht="15.0" customHeight="true">
-      <c r="A3" t="s" s="3">
-        <v>12</v>
-      </c>
       <c r="B3" t="s" s="3">
-        <v>13</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E3" s="3" t="n">
-        <v>20.0</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="C3" t="s" s="3">
+        <v>9</v>
+      </c>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4"/>
+      <c r="G4"/>
+      <c r="H4"/>
     </row>
     <row r="5" ht="15.0" customHeight="true">
-      <c r="A5" t="s" s="3">
+      <c r="B5" t="s" s="3">
         <v>10</v>
       </c>
-      <c r="B5" t="s" s="3">
+      <c r="C5" t="s" s="3">
         <v>11</v>
       </c>
-      <c r="C5" s="3"/>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="B6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6"/>
+      <c r="G6"/>
+      <c r="H6"/>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="B7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7" t="s">
+        <v>22</v>
+      </c>
+      <c r="F7"/>
+      <c r="G7"/>
+      <c r="H7"/>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="B8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" t="s">
+        <v>25</v>
+      </c>
+      <c r="E8" t="s">
+        <v>26</v>
+      </c>
+      <c r="F8"/>
+      <c r="G8"/>
+      <c r="H8"/>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="B9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" t="s">
+        <v>29</v>
+      </c>
+      <c r="E9" t="s">
+        <v>15</v>
+      </c>
+      <c r="F9"/>
+      <c r="G9"/>
+      <c r="H9"/>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="B10" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" t="s">
+        <v>31</v>
+      </c>
+      <c r="D10" t="s">
+        <v>32</v>
+      </c>
+      <c r="E10" t="s">
+        <v>15</v>
+      </c>
+      <c r="F10"/>
+      <c r="G10"/>
+      <c r="H10"/>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="B11" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11" t="s">
+        <v>34</v>
+      </c>
+      <c r="D11" t="s">
+        <v>35</v>
+      </c>
+      <c r="E11" t="s">
+        <v>15</v>
+      </c>
+      <c r="F11"/>
+      <c r="G11"/>
+      <c r="H11"/>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="B12" t="s">
+        <v>36</v>
+      </c>
+      <c r="C12" t="s">
+        <v>37</v>
+      </c>
+      <c r="D12" t="s">
+        <v>38</v>
+      </c>
+      <c r="E12" t="s">
+        <v>15</v>
+      </c>
+      <c r="F12"/>
+      <c r="G12"/>
+      <c r="H12"/>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>8.0</v>
+      </c>
+      <c r="B13" t="s">
+        <v>39</v>
+      </c>
+      <c r="C13" t="s">
+        <v>40</v>
+      </c>
+      <c r="D13" t="s">
+        <v>41</v>
+      </c>
+      <c r="E13" t="s">
+        <v>15</v>
+      </c>
+      <c r="F13"/>
+      <c r="G13"/>
+      <c r="H13"/>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>9.0</v>
+      </c>
+      <c r="B14" t="s">
+        <v>42</v>
+      </c>
+      <c r="C14" t="s">
+        <v>43</v>
+      </c>
+      <c r="D14" t="s">
+        <v>44</v>
+      </c>
+      <c r="E14" t="s">
+        <v>15</v>
+      </c>
+      <c r="F14"/>
+      <c r="G14"/>
+      <c r="H14"/>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="B15" t="s">
+        <v>45</v>
+      </c>
+      <c r="C15" t="s">
+        <v>46</v>
+      </c>
+      <c r="D15" t="s">
+        <v>47</v>
+      </c>
+      <c r="E15" t="s">
+        <v>48</v>
+      </c>
+      <c r="F15"/>
+      <c r="G15"/>
+      <c r="H15"/>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>11.0</v>
+      </c>
+      <c r="B16" t="s">
+        <v>49</v>
+      </c>
+      <c r="C16" t="s">
+        <v>50</v>
+      </c>
+      <c r="D16" t="s">
+        <v>51</v>
+      </c>
+      <c r="E16" t="s">
+        <v>52</v>
+      </c>
+      <c r="F16"/>
+      <c r="G16"/>
+      <c r="H16"/>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="B17" t="s">
+        <v>53</v>
+      </c>
+      <c r="C17" t="s">
+        <v>54</v>
+      </c>
+      <c r="D17" t="s">
+        <v>55</v>
+      </c>
+      <c r="E17" t="s">
+        <v>56</v>
+      </c>
+      <c r="F17"/>
+      <c r="G17"/>
+      <c r="H17"/>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>13.0</v>
+      </c>
+      <c r="B18" t="s">
+        <v>57</v>
+      </c>
+      <c r="C18" t="s">
+        <v>58</v>
+      </c>
+      <c r="D18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E18" t="s">
+        <v>15</v>
+      </c>
+      <c r="F18"/>
+      <c r="G18"/>
+      <c r="H18"/>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>14.0</v>
+      </c>
+      <c r="B19" t="s">
+        <v>60</v>
+      </c>
+      <c r="C19" t="s">
+        <v>61</v>
+      </c>
+      <c r="D19" t="s">
+        <v>62</v>
+      </c>
+      <c r="E19" t="s">
+        <v>63</v>
+      </c>
+      <c r="F19"/>
+      <c r="G19"/>
+      <c r="H19"/>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>15.0</v>
+      </c>
+      <c r="B20" t="s">
+        <v>64</v>
+      </c>
+      <c r="C20" t="s">
+        <v>65</v>
+      </c>
+      <c r="D20" t="s">
+        <v>66</v>
+      </c>
+      <c r="E20" t="s">
+        <v>67</v>
+      </c>
+      <c r="F20"/>
+      <c r="G20"/>
+      <c r="H20"/>
     </row>
   </sheetData>
   <mergeCells>
-    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A1:H1"/>
   </mergeCells>
   <printOptions horizontalCentered="true"/>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>

</xml_diff>

<commit_message>
Correções de melhoria de desempeho.
</commit_message>
<xml_diff>
--- a/ProjetoAlgoritmoDeInferencia/Saída/Percentual de similaridade.xlsx
+++ b/ProjetoAlgoritmoDeInferencia/Saída/Percentual de similaridade.xlsx
@@ -7,6 +7,7 @@
   </bookViews>
   <sheets>
     <sheet name="Percentual de similaridade" r:id="rId3" sheetId="1"/>
+    <sheet name="Percentual de similaridade 2" r:id="rId4" sheetId="2"/>
   </sheets>
 </workbook>
 </file>
@@ -403,7 +404,7 @@
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
     <col min="1" max="1" width="2.0" customWidth="true"/>
-    <col min="2" max="2" width="24.0" customWidth="true"/>
+    <col min="2" max="2" width="26.0" customWidth="true"/>
     <col min="3" max="3" width="20.0" customWidth="true"/>
     <col min="4" max="4" width="18.0" customWidth="true"/>
     <col min="5" max="5" width="20.0" customWidth="true"/>
@@ -795,4 +796,17 @@
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="landscape"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup orientation="landscape"/>
+</worksheet>
 </file>
</xml_diff>